<commit_message>
finished survey monkey project
</commit_message>
<xml_diff>
--- a/data_analysis/survey_mokey_cleaning/Data - Survey Monkey Output.xlsx
+++ b/data_analysis/survey_mokey_cleaning/Data - Survey Monkey Output.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g42v/Documents/Personal/Ad Hoc Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://issdcu-my.sharepoint.com/personal/joseph_oluwasanya2_mail_dcu_ie/Documents/Documents/ds_projects/data_analysis/survey_mokey_cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCD6AED7-7069-C543-93F4-3018A1828479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{DCD6AED7-7069-C543-93F4-3018A1828479}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{333F1637-D62A-415C-98F7-F42E71BCCAA1}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="460" windowWidth="35840" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Desired Format" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17078" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17088" uniqueCount="109">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -337,6 +338,27 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Demographic Info</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Question+Subquestion</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Total Respondents</t>
+  </si>
+  <si>
+    <t>Same Answer</t>
   </si>
 </sst>
 </file>
@@ -751,18 +773,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:100" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -893,7 +915,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:100" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:100" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5379192392</v>
       </c>
@@ -1449,7 +1471,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2658722536</v>
       </c>
@@ -1721,7 +1743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4044163394</v>
       </c>
@@ -1999,7 +2021,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5535865599</v>
       </c>
@@ -2271,7 +2293,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3356802928</v>
       </c>
@@ -2531,7 +2553,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3399511781</v>
       </c>
@@ -2791,7 +2813,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9860597462</v>
       </c>
@@ -3060,7 +3082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1494621946</v>
       </c>
@@ -3323,7 +3345,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8646387163</v>
       </c>
@@ -3583,7 +3605,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2455127238</v>
       </c>
@@ -3855,7 +3877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1905266879</v>
       </c>
@@ -4100,7 +4122,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7089369660</v>
       </c>
@@ -4363,7 +4385,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3397360934</v>
       </c>
@@ -4623,7 +4645,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6904821010</v>
       </c>
@@ -4898,7 +4920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9961006444</v>
       </c>
@@ -5164,7 +5186,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9736526482</v>
       </c>
@@ -5433,7 +5455,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8035211358</v>
       </c>
@@ -5699,7 +5721,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2855503402</v>
       </c>
@@ -5962,7 +5984,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4136037887</v>
       </c>
@@ -6240,7 +6262,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9624253323</v>
       </c>
@@ -6497,7 +6519,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8546027678</v>
       </c>
@@ -6760,7 +6782,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3555213031</v>
       </c>
@@ -7029,7 +7051,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1754220060</v>
       </c>
@@ -7286,7 +7308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9011744859</v>
       </c>
@@ -7546,7 +7568,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5875585727</v>
       </c>
@@ -7812,7 +7834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9051604151</v>
       </c>
@@ -8081,7 +8103,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6573346680</v>
       </c>
@@ -8335,7 +8357,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4383571615</v>
       </c>
@@ -8598,7 +8620,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5850350235</v>
       </c>
@@ -8867,7 +8889,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9526771290</v>
       </c>
@@ -9142,7 +9164,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8531180699</v>
       </c>
@@ -9420,7 +9442,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3087114007</v>
       </c>
@@ -9686,7 +9708,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7901328134</v>
       </c>
@@ -9958,7 +9980,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1321967343</v>
       </c>
@@ -10221,7 +10243,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2206081204</v>
       </c>
@@ -10481,7 +10503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6285875694</v>
       </c>
@@ -10756,7 +10778,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1587370284</v>
       </c>
@@ -11025,7 +11047,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9270992319</v>
       </c>
@@ -11297,7 +11319,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2888589302</v>
       </c>
@@ -11572,7 +11594,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9939738223</v>
       </c>
@@ -11844,7 +11866,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5794920197</v>
       </c>
@@ -12110,7 +12132,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3968415666</v>
       </c>
@@ -12376,7 +12398,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4166850362</v>
       </c>
@@ -12639,7 +12661,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9945822370</v>
       </c>
@@ -12917,7 +12939,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1948472863</v>
       </c>
@@ -13186,7 +13208,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2603687810</v>
       </c>
@@ -13452,7 +13474,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2696474434</v>
       </c>
@@ -13727,7 +13749,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3044612158</v>
       </c>
@@ -13999,7 +14021,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3040325972</v>
       </c>
@@ -14277,7 +14299,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3618961108</v>
       </c>
@@ -14549,7 +14571,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3536054852</v>
       </c>
@@ -14800,7 +14822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4075412109</v>
       </c>
@@ -15063,7 +15085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7481772195</v>
       </c>
@@ -15341,7 +15363,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5044294817</v>
       </c>
@@ -15610,7 +15632,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3120678959</v>
       </c>
@@ -15879,7 +15901,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6316782091</v>
       </c>
@@ -16145,7 +16167,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9489935616</v>
       </c>
@@ -16408,7 +16430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7178840935</v>
       </c>
@@ -16680,7 +16702,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4625088666</v>
       </c>
@@ -16955,7 +16977,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2899153341</v>
       </c>
@@ -17215,7 +17237,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5081486733</v>
       </c>
@@ -17499,7 +17521,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4211032639</v>
       </c>
@@ -17768,7 +17790,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2273018449</v>
       </c>
@@ -18034,7 +18056,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7276390477</v>
       </c>
@@ -18303,7 +18325,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2618791107</v>
       </c>
@@ -18578,7 +18600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9806028857</v>
       </c>
@@ -18841,7 +18863,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4870706994</v>
       </c>
@@ -19119,7 +19141,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5382550855</v>
       </c>
@@ -19394,7 +19416,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5297870739</v>
       </c>
@@ -19663,7 +19685,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9718877248</v>
       </c>
@@ -19935,7 +19957,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8830958949</v>
       </c>
@@ -20195,7 +20217,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7852677398</v>
       </c>
@@ -20470,7 +20492,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9806832932</v>
       </c>
@@ -20739,7 +20761,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5585138853</v>
       </c>
@@ -21005,7 +21027,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8087395217</v>
       </c>
@@ -21265,7 +21287,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5177954332</v>
       </c>
@@ -21537,7 +21559,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1582292985</v>
       </c>
@@ -21791,7 +21813,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2932152777</v>
       </c>
@@ -22057,7 +22079,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1627698070</v>
       </c>
@@ -22317,7 +22339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9748686287</v>
       </c>
@@ -22580,7 +22602,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>7149169711</v>
       </c>
@@ -22858,7 +22880,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6206953310</v>
       </c>
@@ -23130,7 +23152,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9983361274</v>
       </c>
@@ -23393,7 +23415,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8250575077</v>
       </c>
@@ -23650,7 +23672,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9183378071</v>
       </c>
@@ -23910,7 +23932,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>3868607625</v>
       </c>
@@ -24173,7 +24195,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1411900712</v>
       </c>
@@ -24445,7 +24467,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3860289517</v>
       </c>
@@ -24699,7 +24721,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>6014941727</v>
       </c>
@@ -24965,7 +24987,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>9323454815</v>
       </c>
@@ -25243,7 +25265,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="93" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>8311558071</v>
       </c>
@@ -25509,7 +25531,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>7819918439</v>
       </c>
@@ -25778,7 +25800,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2007145908</v>
       </c>
@@ -26047,7 +26069,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5386015734</v>
       </c>
@@ -26322,7 +26344,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2373830201</v>
       </c>
@@ -26588,7 +26610,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>3564004995</v>
       </c>
@@ -26851,7 +26873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4947111306</v>
       </c>
@@ -27126,7 +27148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5078285109</v>
       </c>
@@ -27392,7 +27414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>6225804357</v>
       </c>
@@ -27673,7 +27695,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2014555149</v>
       </c>
@@ -27948,7 +27970,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2243120133</v>
       </c>
@@ -28211,7 +28233,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3550987529</v>
       </c>
@@ -28486,7 +28508,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4228546491</v>
       </c>
@@ -28755,7 +28777,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="106" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2062616124</v>
       </c>
@@ -29030,7 +29052,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>3244391841</v>
       </c>
@@ -29299,7 +29321,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5488107363</v>
       </c>
@@ -29577,7 +29599,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>8585347438</v>
       </c>
@@ -29840,7 +29862,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="110" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7133066581</v>
       </c>
@@ -30109,7 +30131,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2817787256</v>
       </c>
@@ -30381,7 +30403,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1636734067</v>
       </c>
@@ -30656,7 +30678,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="113" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>5202048947</v>
       </c>
@@ -30931,7 +30953,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>3184415812</v>
       </c>
@@ -31212,7 +31234,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="115" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>5157551249</v>
       </c>
@@ -31484,7 +31506,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>9597476932</v>
       </c>
@@ -31753,7 +31775,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>5350663671</v>
       </c>
@@ -32007,7 +32029,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="118" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>7164689614</v>
       </c>
@@ -32282,7 +32304,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>4295285752</v>
       </c>
@@ -32551,7 +32573,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>4008763646</v>
       </c>
@@ -32817,7 +32839,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>6909546929</v>
       </c>
@@ -33080,7 +33102,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="122" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>7331440341</v>
       </c>
@@ -33346,7 +33368,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="123" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>4617669690</v>
       </c>
@@ -33606,7 +33628,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1892199000</v>
       </c>
@@ -33878,7 +33900,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="125" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>7480026174</v>
       </c>
@@ -34141,7 +34163,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="126" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1859209548</v>
       </c>
@@ -34404,7 +34426,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="127" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2065485156</v>
       </c>
@@ -34676,7 +34698,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="128" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8008971893</v>
       </c>
@@ -34942,7 +34964,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="129" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1967962301</v>
       </c>
@@ -35217,7 +35239,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="130" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>8708081021</v>
       </c>
@@ -35483,7 +35505,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="131" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>9462494279</v>
       </c>
@@ -35740,7 +35762,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2126438547</v>
       </c>
@@ -36006,7 +36028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>8748263039</v>
       </c>
@@ -36278,7 +36300,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="134" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>4366243452</v>
       </c>
@@ -36559,7 +36581,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="135" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1368436554</v>
       </c>
@@ -36828,7 +36850,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="136" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>6588311032</v>
       </c>
@@ -37073,7 +37095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>9652438783</v>
       </c>
@@ -37345,7 +37367,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="138" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>8895572278</v>
       </c>
@@ -37608,7 +37630,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="139" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>5633495172</v>
       </c>
@@ -37868,7 +37890,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="140" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6665212340</v>
       </c>
@@ -38134,7 +38156,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2850296334</v>
       </c>
@@ -38394,7 +38416,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="142" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2781168270</v>
       </c>
@@ -38672,7 +38694,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="143" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>6478560213</v>
       </c>
@@ -38941,7 +38963,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>9328885416</v>
       </c>
@@ -39213,7 +39235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="145" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6285007368</v>
       </c>
@@ -39476,7 +39498,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="146" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>6776579131</v>
       </c>
@@ -39745,7 +39767,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="147" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6270834102</v>
       </c>
@@ -39996,7 +40018,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="148" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>4341029891</v>
       </c>
@@ -40259,7 +40281,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="149" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>9298970467</v>
       </c>
@@ -40531,7 +40553,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="150" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>3530464299</v>
       </c>
@@ -40800,7 +40822,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="151" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1962504465</v>
       </c>
@@ -41054,7 +41076,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="152" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>3206389468</v>
       </c>
@@ -41317,7 +41339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="153" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1914548336</v>
       </c>
@@ -41595,7 +41617,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="154" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>6912636653</v>
       </c>
@@ -41855,7 +41877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="155" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>7447366993</v>
       </c>
@@ -42121,7 +42143,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="156" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>9858203307</v>
       </c>
@@ -42393,7 +42415,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="157" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2375491161</v>
       </c>
@@ -42659,7 +42681,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="158" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>6983214026</v>
       </c>
@@ -42943,7 +42965,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="159" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>7876887860</v>
       </c>
@@ -43209,7 +43231,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="160" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>5282809243</v>
       </c>
@@ -43466,7 +43488,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="161" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>4304756587</v>
       </c>
@@ -43732,7 +43754,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="162" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>6841338036</v>
       </c>
@@ -43989,7 +44011,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1338692945</v>
       </c>
@@ -44261,7 +44283,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1220878407</v>
       </c>
@@ -44527,7 +44549,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="165" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1021794253</v>
       </c>
@@ -44802,7 +44824,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="166" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>7103482882</v>
       </c>
@@ -45065,7 +45087,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>6080354155</v>
       </c>
@@ -45337,7 +45359,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="168" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>8046048988</v>
       </c>
@@ -45612,7 +45634,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="169" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2102054017</v>
       </c>
@@ -45884,7 +45906,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>6796580906</v>
       </c>
@@ -46141,7 +46163,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="171" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>3966690436</v>
       </c>
@@ -46398,7 +46420,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="172" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>8630148625</v>
       </c>
@@ -46664,7 +46686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="173" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1264208927</v>
       </c>
@@ -46930,7 +46952,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="174" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>9625886165</v>
       </c>
@@ -47199,7 +47221,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="175" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>9351204267</v>
       </c>
@@ -47477,7 +47499,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="176" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1485638866</v>
       </c>
@@ -47743,7 +47765,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="177" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>9137601822</v>
       </c>
@@ -48009,7 +48031,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="178" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>4910729713</v>
       </c>
@@ -48269,7 +48291,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="179" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>8453428178</v>
       </c>
@@ -48541,7 +48563,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="180" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>6903105973</v>
       </c>
@@ -48816,7 +48838,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="181" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2628194343</v>
       </c>
@@ -49079,7 +49101,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="182" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2254451126</v>
       </c>
@@ -49351,7 +49373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="183" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1426184525</v>
       </c>
@@ -49623,7 +49645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="184" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1001882880</v>
       </c>
@@ -49901,7 +49923,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="185" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1941311372</v>
       </c>
@@ -50155,7 +50177,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="186" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>8569413026</v>
       </c>
@@ -50427,7 +50449,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="187" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>5953471955</v>
       </c>
@@ -50693,7 +50715,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="188" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>3933988341</v>
       </c>
@@ -50959,7 +50981,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="189" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>7963965247</v>
       </c>
@@ -51225,7 +51247,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="190" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>9735550076</v>
       </c>
@@ -51506,7 +51528,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="191" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>5559071396</v>
       </c>
@@ -51778,7 +51800,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="192" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>8253262223</v>
       </c>
@@ -52053,7 +52075,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="193" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>7325851635</v>
       </c>
@@ -52319,7 +52341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="194" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>3370365802</v>
       </c>
@@ -52588,7 +52610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="195" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2841747833</v>
       </c>
@@ -52854,7 +52876,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="196" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>7940065082</v>
       </c>
@@ -53123,7 +53145,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="197" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>5157705612</v>
       </c>
@@ -53401,7 +53423,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="198" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>9920755555</v>
       </c>
@@ -53655,7 +53677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="199" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>6638341389</v>
       </c>
@@ -53921,7 +53943,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="200" spans="1:100" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>8114622230</v>
       </c>
@@ -54182,4 +54204,56 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3639FF91-45F2-42A1-8087-C3BD4FA83736}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>